<commit_message>
Edit Gestion sem 6
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine6.xlsx
+++ b/meeting/GestionHedbo_Semaine6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Objet de la réunion : Hebdomadaire</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Test unitaire</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Fixer caméra robot</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t>Imane</t>
-  </si>
-  <si>
-    <t>Détection Kinect</t>
   </si>
   <si>
     <t>Plan d'intégration</t>
@@ -235,7 +229,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,12 +256,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -286,8 +274,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -406,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -455,7 +443,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -463,65 +450,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -896,7 +890,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E47" sqref="E47:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -907,10 +901,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -919,12 +913,12 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -945,15 +939,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -963,45 +957,45 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32" t="s">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1015,15 +1009,15 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1051,7 +1045,7 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1060,21 +1054,21 @@
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="48">
+      <c r="D12" s="24"/>
+      <c r="E12" s="31">
         <v>150</v>
       </c>
       <c r="F12" s="10">
         <v>12</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="28">
         <f>E12-SUM(F12:F12)</f>
         <v>138</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1083,95 +1077,95 @@
       <c r="C13" s="9">
         <v>41336</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="39">
+      <c r="D13" s="23"/>
+      <c r="E13" s="32">
         <v>150</v>
       </c>
       <c r="F13" s="10">
         <v>2</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="42">
         <f>(E13-SUM(F13:F17))</f>
         <v>138</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="9">
         <v>41336</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="40"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="10">
         <v>1</v>
       </c>
-      <c r="G14" s="34"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="40"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="10">
         <v>3</v>
       </c>
-      <c r="G15" s="34"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="9">
         <v>41336</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="40"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="10">
         <v>1</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="40"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="10">
         <v>5</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="41"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="34"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1180,69 +1174,69 @@
       <c r="C19" s="9">
         <v>41336</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="39">
+      <c r="D19" s="25"/>
+      <c r="E19" s="32">
         <v>142</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="35">
         <f>E19-SUM(F19:F22)</f>
         <v>132</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="40"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="10">
         <v>2</v>
       </c>
-      <c r="G20" s="44"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="9">
         <v>41336</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="40"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="10">
         <v>3</v>
       </c>
-      <c r="G21" s="44"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="9">
         <v>41489</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="41"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="34"/>
       <c r="F22" s="10">
         <v>4</v>
       </c>
-      <c r="G22" s="45"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1251,310 +1245,296 @@
       <c r="C23" s="9">
         <v>41336</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="34">
+      <c r="D23" s="25"/>
+      <c r="E23" s="42">
         <v>136</v>
       </c>
       <c r="F23" s="10">
         <v>1</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="42">
         <f>E23-SUM(F23:F26)</f>
         <v>127</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="9">
-        <v>41336</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="34"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="10">
         <v>3</v>
       </c>
-      <c r="G24" s="34"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="10">
         <v>2</v>
       </c>
-      <c r="G25" s="34"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="9">
         <v>41336</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="34"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="10">
         <v>3</v>
       </c>
-      <c r="G26" s="34"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="34"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="18">
         <v>1</v>
       </c>
-      <c r="G27" s="34"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="34"/>
+        <v>35</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="14">
         <v>6</v>
       </c>
-      <c r="G28" s="34"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="35">
+        <v>35</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="43">
         <v>137</v>
       </c>
       <c r="F29" s="10">
         <v>10</v>
       </c>
-      <c r="G29" s="35">
+      <c r="G29" s="43">
         <f>(E29)-SUM(F29:F33)</f>
         <v>118</v>
       </c>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="9">
-        <v>41336</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="35"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="10">
         <v>3</v>
       </c>
-      <c r="G30" s="35"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="35"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="10">
         <v>2</v>
       </c>
-      <c r="G31" s="35"/>
+      <c r="G31" s="43"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="9">
         <v>41336</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="10">
         <v>1</v>
       </c>
-      <c r="G32" s="35"/>
+      <c r="G32" s="43"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="9">
         <v>41336</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="35"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="43"/>
       <c r="F33" s="10">
         <v>3</v>
       </c>
-      <c r="G33" s="35"/>
+      <c r="G33" s="43"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="35">
+      <c r="A34" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="43">
         <v>119</v>
       </c>
       <c r="F34" s="10">
         <v>6</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G34" s="43">
         <f>(E34)-SUM(F34:F40)</f>
         <v>97</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="9">
         <v>41336</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="35"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="10">
         <v>3</v>
       </c>
-      <c r="G35" s="35"/>
+      <c r="G35" s="43"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="35"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="10">
         <v>2</v>
       </c>
-      <c r="G36" s="35"/>
+      <c r="G36" s="43"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="9">
         <v>41336</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="35"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="10">
         <v>1</v>
       </c>
-      <c r="G37" s="35"/>
+      <c r="G37" s="43"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="9">
         <v>41336</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="35"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="10">
         <v>3</v>
       </c>
-      <c r="G38" s="35"/>
+      <c r="G38" s="43"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="9">
         <v>41336</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="35"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="43"/>
       <c r="F39" s="10">
         <v>4</v>
       </c>
-      <c r="G39" s="35"/>
+      <c r="G39" s="43"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" s="9">
         <v>41336</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="35"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="43"/>
       <c r="F40" s="10">
         <v>3</v>
       </c>
-      <c r="G40" s="35"/>
+      <c r="G40" s="43"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
-        <v>44</v>
+      <c r="A41" s="43" t="s">
+        <v>42</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>32</v>
@@ -1562,226 +1542,226 @@
       <c r="C41" s="9">
         <v>41336</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="34">
+      <c r="D41" s="23"/>
+      <c r="E41" s="42">
         <v>124</v>
       </c>
       <c r="F41" s="10">
         <v>3</v>
       </c>
-      <c r="G41" s="34">
+      <c r="G41" s="42">
         <f>E41-SUM(F41:F46)</f>
         <v>108</v>
       </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="9">
         <v>41336</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="34"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="42"/>
       <c r="F42" s="10">
         <v>1</v>
       </c>
-      <c r="G42" s="34"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="34"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="42"/>
       <c r="F43" s="10">
         <v>2</v>
       </c>
-      <c r="G43" s="34"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="42"/>
       <c r="F44" s="10">
         <v>4</v>
       </c>
-      <c r="G44" s="34"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" s="9">
         <v>41336</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="34"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="10">
         <v>4</v>
       </c>
-      <c r="G45" s="34"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="9">
         <v>41336</v>
       </c>
-      <c r="D46" s="25"/>
-      <c r="E46" s="34"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="42"/>
       <c r="F46" s="10">
         <v>2</v>
       </c>
-      <c r="G46" s="34"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
-        <v>49</v>
+      <c r="A47" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="9">
         <v>41336</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="34">
+      <c r="D47" s="48"/>
+      <c r="E47" s="42">
         <v>130</v>
       </c>
       <c r="F47" s="10">
         <v>3</v>
       </c>
-      <c r="G47" s="34">
+      <c r="G47" s="42">
         <f>E47-SUM(F47:F53)</f>
         <v>115</v>
       </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="9">
         <v>41336</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="34"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="42"/>
       <c r="F48" s="10">
         <v>1</v>
       </c>
-      <c r="G48" s="34"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="34"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="42"/>
       <c r="F49" s="10">
         <v>2</v>
       </c>
-      <c r="G49" s="34"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
+      <c r="A50" s="42"/>
       <c r="B50" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="9">
         <v>41336</v>
       </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="34"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="42"/>
       <c r="F50" s="10">
         <v>3</v>
       </c>
-      <c r="G50" s="34"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" s="9">
         <v>41336</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="34"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="42"/>
       <c r="F51" s="10">
         <v>4</v>
       </c>
-      <c r="G51" s="34"/>
+      <c r="G51" s="42"/>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" s="19"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="34"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="42"/>
       <c r="F52" s="10">
         <v>2</v>
       </c>
-      <c r="G52" s="34"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
+      <c r="A53" s="42"/>
       <c r="B53" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="G53" s="42"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="10" t="s">
+      <c r="B54" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="34"/>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="37"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="22">
+      <c r="E54" s="21">
         <f>SUM(E12:E22)</f>
         <v>442</v>
       </c>
@@ -1790,15 +1770,15 @@
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="37"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="22">
+      <c r="E55" s="21">
         <f>SUM(E23:E40)</f>
         <v>392</v>
       </c>
@@ -1807,15 +1787,15 @@
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C56" s="37"/>
+      <c r="A56" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="39"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="22">
+      <c r="E56" s="21">
         <f>SUM(E41:E52)</f>
         <v>254</v>
       </c>
@@ -1824,13 +1804,13 @@
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
+      <c r="A57" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
       <c r="D57" s="6"/>
-      <c r="E57" s="22">
+      <c r="E57" s="21">
         <f>SUM(E54:E56)</f>
         <v>1088</v>
       </c>
@@ -1845,75 +1825,75 @@
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="23"/>
+      <c r="G58" s="22"/>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
+      <c r="A59" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
+      <c r="C60" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="38"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="38"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1928,11 +1908,28 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="G13:G18"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="G29:G33"/>
     <mergeCell ref="C64:G64"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
@@ -1940,6 +1937,11 @@
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="C60:G61"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C63:G63"/>
     <mergeCell ref="A47:A53"/>
     <mergeCell ref="E47:E53"/>
     <mergeCell ref="G47:G53"/>
@@ -1951,28 +1953,6 @@
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="E41:E46"/>
     <mergeCell ref="G41:G46"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="G13:G18"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>